<commit_message>
added a second bar graph - good working prototype
</commit_message>
<xml_diff>
--- a/external_input/input.xlsx
+++ b/external_input/input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wogie\Desktop\Projects React Course\Bitcoin stuff\SciBit\scibit\external_input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCFCC5F8-08E9-482F-845F-C90FF5A17426}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D5CCAE0-C356-4AA2-8281-C365C3CF9DDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38295" yWindow="-1125" windowWidth="20565" windowHeight="16290" xr2:uid="{3A017B69-62D2-4043-87B6-99B82A75BBCF}"/>
+    <workbookView xWindow="-19215" yWindow="-1695" windowWidth="17835" windowHeight="16290" xr2:uid="{3A017B69-62D2-4043-87B6-99B82A75BBCF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="4" r:id="rId1"/>
@@ -800,11 +800,137 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{490F86A6-FCF6-4696-9B4F-F1627DA98DEB}">
   <dimension ref="A1:DX14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="W1" sqref="W1:W1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.77734375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6.77734375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="7" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5.77734375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="6.77734375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="5.77734375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="6.77734375" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="3.5546875" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="11" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="8" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="4.44140625" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="6.77734375" bestFit="1" customWidth="1"/>
+    <col min="61" max="62" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="16" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="8" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="6" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="6.21875" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="7.77734375" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="5.21875" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="6.77734375" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="10" bestFit="1" customWidth="1"/>
+    <col min="77" max="78" width="5.77734375" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="10" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="4.44140625" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="9" bestFit="1" customWidth="1"/>
+    <col min="89" max="89" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="90" max="90" width="6.77734375" bestFit="1" customWidth="1"/>
+    <col min="91" max="91" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="93" max="93" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="94" max="94" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="95" max="95" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="96" max="96" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="97" max="97" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="98" max="98" width="8" bestFit="1" customWidth="1"/>
+    <col min="99" max="99" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="100" max="100" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="101" max="101" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="102" max="102" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="103" max="103" width="8" bestFit="1" customWidth="1"/>
+    <col min="104" max="104" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="105" max="105" width="9" bestFit="1" customWidth="1"/>
+    <col min="106" max="106" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="107" max="107" width="19" bestFit="1" customWidth="1"/>
+    <col min="108" max="108" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="109" max="109" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="110" max="110" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="111" max="111" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="112" max="112" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="113" max="113" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="114" max="114" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="115" max="115" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="116" max="116" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="117" max="117" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="118" max="118" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="119" max="119" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="120" max="120" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="121" max="121" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="123" max="123" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="124" max="124" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="125" max="125" width="6.77734375" bestFit="1" customWidth="1"/>
+    <col min="126" max="126" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="127" max="127" width="7.77734375" bestFit="1" customWidth="1"/>
+    <col min="128" max="128" width="7.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:128" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -840,7 +966,7 @@
       <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
       <c r="M1" t="s">
@@ -852,7 +978,7 @@
       <c r="O1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
       <c r="Q1" t="s">
@@ -873,7 +999,7 @@
       <c r="V1" t="s">
         <v>20</v>
       </c>
-      <c r="W1" t="s">
+      <c r="W1" s="1" t="s">
         <v>21</v>
       </c>
       <c r="X1" t="s">
@@ -1226,7 +1352,7 @@
       <c r="K2">
         <v>0</v>
       </c>
-      <c r="L2">
+      <c r="L2" s="1">
         <v>0</v>
       </c>
       <c r="M2">
@@ -1238,7 +1364,7 @@
       <c r="O2">
         <v>0</v>
       </c>
-      <c r="P2">
+      <c r="P2" s="1">
         <v>0</v>
       </c>
       <c r="Q2">
@@ -1259,7 +1385,7 @@
       <c r="V2">
         <v>0</v>
       </c>
-      <c r="W2">
+      <c r="W2" s="1">
         <v>0</v>
       </c>
       <c r="X2">
@@ -1612,7 +1738,7 @@
       <c r="K3">
         <v>0</v>
       </c>
-      <c r="L3">
+      <c r="L3" s="1">
         <v>0</v>
       </c>
       <c r="M3">
@@ -1624,7 +1750,7 @@
       <c r="O3">
         <v>0</v>
       </c>
-      <c r="P3">
+      <c r="P3" s="1">
         <v>0</v>
       </c>
       <c r="Q3">
@@ -1645,7 +1771,7 @@
       <c r="V3">
         <v>0</v>
       </c>
-      <c r="W3">
+      <c r="W3" s="1">
         <v>0</v>
       </c>
       <c r="X3">
@@ -1998,7 +2124,7 @@
       <c r="K4">
         <v>1</v>
       </c>
-      <c r="L4">
+      <c r="L4" s="1">
         <v>1</v>
       </c>
       <c r="M4">
@@ -2010,7 +2136,7 @@
       <c r="O4">
         <v>1</v>
       </c>
-      <c r="P4">
+      <c r="P4" s="1">
         <v>1</v>
       </c>
       <c r="Q4">
@@ -2031,7 +2157,7 @@
       <c r="V4">
         <v>0</v>
       </c>
-      <c r="W4">
+      <c r="W4" s="1">
         <v>0</v>
       </c>
       <c r="X4">
@@ -2384,7 +2510,7 @@
       <c r="K5">
         <v>3</v>
       </c>
-      <c r="L5">
+      <c r="L5" s="1">
         <v>2</v>
       </c>
       <c r="M5">
@@ -2396,7 +2522,7 @@
       <c r="O5">
         <v>4</v>
       </c>
-      <c r="P5">
+      <c r="P5" s="1">
         <v>1</v>
       </c>
       <c r="Q5">
@@ -2417,7 +2543,7 @@
       <c r="V5">
         <v>2</v>
       </c>
-      <c r="W5">
+      <c r="W5" s="1">
         <v>2</v>
       </c>
       <c r="X5">
@@ -2770,7 +2896,7 @@
       <c r="K6">
         <v>6</v>
       </c>
-      <c r="L6">
+      <c r="L6" s="1">
         <v>2</v>
       </c>
       <c r="M6">
@@ -2782,7 +2908,7 @@
       <c r="O6">
         <v>8</v>
       </c>
-      <c r="P6">
+      <c r="P6" s="1">
         <v>0</v>
       </c>
       <c r="Q6">
@@ -2803,7 +2929,7 @@
       <c r="V6">
         <v>0</v>
       </c>
-      <c r="W6">
+      <c r="W6" s="1">
         <v>0</v>
       </c>
       <c r="X6">
@@ -3156,7 +3282,7 @@
       <c r="K7">
         <v>11</v>
       </c>
-      <c r="L7">
+      <c r="L7" s="1">
         <v>12</v>
       </c>
       <c r="M7">
@@ -3168,7 +3294,7 @@
       <c r="O7">
         <v>2</v>
       </c>
-      <c r="P7">
+      <c r="P7" s="1">
         <v>3</v>
       </c>
       <c r="Q7">
@@ -3189,7 +3315,7 @@
       <c r="V7">
         <v>0</v>
       </c>
-      <c r="W7">
+      <c r="W7" s="1">
         <v>4</v>
       </c>
       <c r="X7">
@@ -3542,7 +3668,7 @@
       <c r="K8">
         <v>14</v>
       </c>
-      <c r="L8">
+      <c r="L8" s="1">
         <v>54</v>
       </c>
       <c r="M8">
@@ -3554,7 +3680,7 @@
       <c r="O8">
         <v>12</v>
       </c>
-      <c r="P8">
+      <c r="P8" s="1">
         <v>3</v>
       </c>
       <c r="Q8">
@@ -3575,7 +3701,7 @@
       <c r="V8">
         <v>0</v>
       </c>
-      <c r="W8">
+      <c r="W8" s="1">
         <v>4</v>
       </c>
       <c r="X8">
@@ -3928,7 +4054,7 @@
       <c r="K9">
         <v>27</v>
       </c>
-      <c r="L9">
+      <c r="L9" s="1">
         <v>127</v>
       </c>
       <c r="M9">
@@ -3940,7 +4066,7 @@
       <c r="O9">
         <v>11</v>
       </c>
-      <c r="P9">
+      <c r="P9" s="1">
         <v>11</v>
       </c>
       <c r="Q9">
@@ -3961,7 +4087,7 @@
       <c r="V9">
         <v>1</v>
       </c>
-      <c r="W9">
+      <c r="W9" s="1">
         <v>7</v>
       </c>
       <c r="X9">
@@ -4314,7 +4440,7 @@
       <c r="K10">
         <v>72</v>
       </c>
-      <c r="L10">
+      <c r="L10" s="1">
         <v>211</v>
       </c>
       <c r="M10">
@@ -4326,7 +4452,7 @@
       <c r="O10">
         <v>7</v>
       </c>
-      <c r="P10">
+      <c r="P10" s="1">
         <v>10</v>
       </c>
       <c r="Q10">
@@ -4347,7 +4473,7 @@
       <c r="V10">
         <v>4</v>
       </c>
-      <c r="W10">
+      <c r="W10" s="1">
         <v>17</v>
       </c>
       <c r="X10">
@@ -4700,7 +4826,7 @@
       <c r="K11">
         <v>52</v>
       </c>
-      <c r="L11">
+      <c r="L11" s="1">
         <v>240</v>
       </c>
       <c r="M11">
@@ -4712,7 +4838,7 @@
       <c r="O11">
         <v>11</v>
       </c>
-      <c r="P11">
+      <c r="P11" s="1">
         <v>6</v>
       </c>
       <c r="Q11">
@@ -4733,7 +4859,7 @@
       <c r="V11">
         <v>4</v>
       </c>
-      <c r="W11">
+      <c r="W11" s="1">
         <v>18</v>
       </c>
       <c r="X11">
@@ -5086,7 +5212,7 @@
       <c r="K12">
         <v>54</v>
       </c>
-      <c r="L12">
+      <c r="L12" s="1">
         <v>295</v>
       </c>
       <c r="M12">
@@ -5098,7 +5224,7 @@
       <c r="O12">
         <v>17</v>
       </c>
-      <c r="P12">
+      <c r="P12" s="1">
         <v>11</v>
       </c>
       <c r="Q12">
@@ -5119,7 +5245,7 @@
       <c r="V12">
         <v>3</v>
       </c>
-      <c r="W12">
+      <c r="W12" s="1">
         <v>28</v>
       </c>
       <c r="X12">
@@ -5472,7 +5598,7 @@
       <c r="K13">
         <v>67</v>
       </c>
-      <c r="L13">
+      <c r="L13" s="1">
         <v>379</v>
       </c>
       <c r="M13">
@@ -5484,7 +5610,7 @@
       <c r="O13">
         <v>15</v>
       </c>
-      <c r="P13">
+      <c r="P13" s="1">
         <v>4</v>
       </c>
       <c r="Q13">
@@ -5505,7 +5631,7 @@
       <c r="V13">
         <v>9</v>
       </c>
-      <c r="W13">
+      <c r="W13" s="1">
         <v>32</v>
       </c>
       <c r="X13">
@@ -5858,7 +5984,7 @@
       <c r="K14">
         <v>60</v>
       </c>
-      <c r="L14">
+      <c r="L14" s="1">
         <v>328</v>
       </c>
       <c r="M14">
@@ -5870,7 +5996,7 @@
       <c r="O14">
         <v>12</v>
       </c>
-      <c r="P14">
+      <c r="P14" s="1">
         <v>6</v>
       </c>
       <c r="Q14">
@@ -5891,7 +6017,7 @@
       <c r="V14">
         <v>9</v>
       </c>
-      <c r="W14">
+      <c r="W14" s="1">
         <v>27</v>
       </c>
       <c r="X14">

</xml_diff>

<commit_message>
finished all countries with Wercia
</commit_message>
<xml_diff>
--- a/external_input/input.xlsx
+++ b/external_input/input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wogie\Desktop\Projects React Course\Bitcoin stuff\SciBit\scibit\external_input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D5CCAE0-C356-4AA2-8281-C365C3CF9DDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9C449BE-FCD9-4216-9077-C6CFCFF54440}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19215" yWindow="-1695" windowWidth="17835" windowHeight="16290" xr2:uid="{3A017B69-62D2-4043-87B6-99B82A75BBCF}"/>
+    <workbookView xWindow="-48060" yWindow="-2205" windowWidth="17835" windowHeight="16290" xr2:uid="{3A017B69-62D2-4043-87B6-99B82A75BBCF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="4" r:id="rId1"/>
@@ -435,7 +435,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -445,6 +445,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -461,9 +467,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -800,8 +807,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{490F86A6-FCF6-4696-9B4F-F1627DA98DEB}">
   <dimension ref="A1:DX14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="W1" sqref="W1:W1048576"/>
+    <sheetView tabSelected="1" topLeftCell="BK1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="BQ18" sqref="BQ18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -841,13 +848,13 @@
     <col min="33" max="33" width="6.77734375" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="11.21875" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="8.77734375" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="6.33203125" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="7.33203125" bestFit="1" customWidth="1"/>
     <col min="40" max="40" width="7.21875" bestFit="1" customWidth="1"/>
     <col min="41" max="41" width="3.5546875" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="11" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="11" style="1" bestFit="1" customWidth="1"/>
     <col min="43" max="43" width="8.33203125" bestFit="1" customWidth="1"/>
     <col min="44" max="44" width="8.77734375" bestFit="1" customWidth="1"/>
     <col min="45" max="45" width="11.21875" bestFit="1" customWidth="1"/>
@@ -859,26 +866,27 @@
     <col min="51" max="51" width="7.33203125" bestFit="1" customWidth="1"/>
     <col min="52" max="52" width="4.44140625" bestFit="1" customWidth="1"/>
     <col min="53" max="53" width="6.88671875" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="8.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="55" max="55" width="12.109375" bestFit="1" customWidth="1"/>
     <col min="56" max="56" width="7.21875" bestFit="1" customWidth="1"/>
     <col min="57" max="57" width="11.88671875" bestFit="1" customWidth="1"/>
     <col min="58" max="58" width="7.21875" bestFit="1" customWidth="1"/>
     <col min="59" max="59" width="6.5546875" bestFit="1" customWidth="1"/>
     <col min="60" max="60" width="6.77734375" bestFit="1" customWidth="1"/>
-    <col min="61" max="62" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="8.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="8.21875" bestFit="1" customWidth="1"/>
     <col min="63" max="63" width="9.109375" bestFit="1" customWidth="1"/>
     <col min="64" max="64" width="5.44140625" bestFit="1" customWidth="1"/>
     <col min="65" max="65" width="8.33203125" bestFit="1" customWidth="1"/>
     <col min="66" max="66" width="16" bestFit="1" customWidth="1"/>
     <col min="67" max="67" width="4.88671875" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="8.44140625" style="2" bestFit="1" customWidth="1"/>
     <col min="69" max="69" width="8" bestFit="1" customWidth="1"/>
     <col min="70" max="70" width="11.109375" bestFit="1" customWidth="1"/>
     <col min="71" max="71" width="6" bestFit="1" customWidth="1"/>
     <col min="72" max="72" width="6.21875" bestFit="1" customWidth="1"/>
     <col min="73" max="73" width="7.77734375" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="5.21875" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="5.21875" style="1" bestFit="1" customWidth="1"/>
     <col min="75" max="75" width="6.77734375" bestFit="1" customWidth="1"/>
     <col min="76" max="76" width="10" bestFit="1" customWidth="1"/>
     <col min="77" max="78" width="5.77734375" bestFit="1" customWidth="1"/>
@@ -889,7 +897,7 @@
     <col min="83" max="83" width="8.21875" bestFit="1" customWidth="1"/>
     <col min="84" max="84" width="11.109375" bestFit="1" customWidth="1"/>
     <col min="85" max="85" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="86" max="86" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="87" max="87" width="8.77734375" bestFit="1" customWidth="1"/>
     <col min="88" max="88" width="9" bestFit="1" customWidth="1"/>
     <col min="89" max="89" width="8.21875" bestFit="1" customWidth="1"/>
@@ -898,7 +906,7 @@
     <col min="93" max="93" width="11.21875" bestFit="1" customWidth="1"/>
     <col min="94" max="94" width="21.88671875" bestFit="1" customWidth="1"/>
     <col min="95" max="95" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="96" max="96" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="96" max="96" width="6.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="97" max="97" width="6.109375" bestFit="1" customWidth="1"/>
     <col min="98" max="98" width="8" bestFit="1" customWidth="1"/>
     <col min="99" max="99" width="10.44140625" bestFit="1" customWidth="1"/>
@@ -910,7 +918,7 @@
     <col min="105" max="105" width="9" bestFit="1" customWidth="1"/>
     <col min="106" max="106" width="11.21875" bestFit="1" customWidth="1"/>
     <col min="107" max="107" width="19" bestFit="1" customWidth="1"/>
-    <col min="108" max="108" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="108" max="108" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="109" max="109" width="12.21875" bestFit="1" customWidth="1"/>
     <col min="110" max="110" width="6.109375" bestFit="1" customWidth="1"/>
     <col min="111" max="111" width="5.44140625" bestFit="1" customWidth="1"/>
@@ -923,7 +931,7 @@
     <col min="118" max="118" width="7.88671875" bestFit="1" customWidth="1"/>
     <col min="119" max="119" width="9.44140625" bestFit="1" customWidth="1"/>
     <col min="120" max="120" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="121" max="121" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="121" max="121" width="11.21875" style="1" bestFit="1" customWidth="1"/>
     <col min="123" max="123" width="4.6640625" bestFit="1" customWidth="1"/>
     <col min="124" max="124" width="6.6640625" bestFit="1" customWidth="1"/>
     <col min="125" max="125" width="6.77734375" bestFit="1" customWidth="1"/>
@@ -1038,7 +1046,7 @@
       <c r="AI1" t="s">
         <v>33</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>34</v>
       </c>
       <c r="AK1" t="s">
@@ -1056,7 +1064,7 @@
       <c r="AO1" t="s">
         <v>39</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>40</v>
       </c>
       <c r="AQ1" t="s">
@@ -1092,7 +1100,7 @@
       <c r="BA1" t="s">
         <v>50</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BB1" s="1" t="s">
         <v>112</v>
       </c>
       <c r="BC1" t="s">
@@ -1113,7 +1121,7 @@
       <c r="BH1" t="s">
         <v>56</v>
       </c>
-      <c r="BI1" t="s">
+      <c r="BI1" s="1" t="s">
         <v>57</v>
       </c>
       <c r="BJ1" t="s">
@@ -1134,7 +1142,7 @@
       <c r="BO1" t="s">
         <v>63</v>
       </c>
-      <c r="BP1" t="s">
+      <c r="BP1" s="2" t="s">
         <v>64</v>
       </c>
       <c r="BQ1" t="s">
@@ -1152,7 +1160,7 @@
       <c r="BU1" t="s">
         <v>69</v>
       </c>
-      <c r="BV1" t="s">
+      <c r="BV1" s="1" t="s">
         <v>70</v>
       </c>
       <c r="BW1" t="s">
@@ -1188,7 +1196,7 @@
       <c r="CG1" t="s">
         <v>81</v>
       </c>
-      <c r="CH1" t="s">
+      <c r="CH1" s="1" t="s">
         <v>82</v>
       </c>
       <c r="CI1" t="s">
@@ -1218,7 +1226,7 @@
       <c r="CQ1" t="s">
         <v>91</v>
       </c>
-      <c r="CR1" t="s">
+      <c r="CR1" s="1" t="s">
         <v>92</v>
       </c>
       <c r="CS1" t="s">
@@ -1254,7 +1262,7 @@
       <c r="DC1" t="s">
         <v>103</v>
       </c>
-      <c r="DD1" t="s">
+      <c r="DD1" s="1" t="s">
         <v>104</v>
       </c>
       <c r="DE1" t="s">
@@ -1293,7 +1301,7 @@
       <c r="DP1" t="s">
         <v>118</v>
       </c>
-      <c r="DQ1" t="s">
+      <c r="DQ1" s="1" t="s">
         <v>119</v>
       </c>
       <c r="DR1" t="s">
@@ -1424,7 +1432,7 @@
       <c r="AI2">
         <v>0</v>
       </c>
-      <c r="AJ2">
+      <c r="AJ2" s="1">
         <v>0</v>
       </c>
       <c r="AK2">
@@ -1442,7 +1450,7 @@
       <c r="AO2">
         <v>0</v>
       </c>
-      <c r="AP2">
+      <c r="AP2" s="1">
         <v>0</v>
       </c>
       <c r="AQ2">
@@ -1478,7 +1486,7 @@
       <c r="BA2">
         <v>0</v>
       </c>
-      <c r="BB2">
+      <c r="BB2" s="1">
         <v>0</v>
       </c>
       <c r="BC2">
@@ -1499,7 +1507,7 @@
       <c r="BH2">
         <v>0</v>
       </c>
-      <c r="BI2">
+      <c r="BI2" s="1">
         <v>0</v>
       </c>
       <c r="BJ2">
@@ -1520,7 +1528,7 @@
       <c r="BO2">
         <v>0</v>
       </c>
-      <c r="BP2">
+      <c r="BP2" s="2">
         <v>0</v>
       </c>
       <c r="BQ2">
@@ -1538,7 +1546,7 @@
       <c r="BU2">
         <v>0</v>
       </c>
-      <c r="BV2">
+      <c r="BV2" s="1">
         <v>0</v>
       </c>
       <c r="BW2">
@@ -1574,7 +1582,7 @@
       <c r="CG2">
         <v>0</v>
       </c>
-      <c r="CH2">
+      <c r="CH2" s="1">
         <v>0</v>
       </c>
       <c r="CI2">
@@ -1604,7 +1612,7 @@
       <c r="CQ2">
         <v>0</v>
       </c>
-      <c r="CR2">
+      <c r="CR2" s="1">
         <v>0</v>
       </c>
       <c r="CS2">
@@ -1640,7 +1648,7 @@
       <c r="DC2">
         <v>0</v>
       </c>
-      <c r="DD2">
+      <c r="DD2" s="1">
         <v>0</v>
       </c>
       <c r="DE2">
@@ -1679,7 +1687,7 @@
       <c r="DP2">
         <v>0</v>
       </c>
-      <c r="DQ2">
+      <c r="DQ2" s="1">
         <v>0</v>
       </c>
       <c r="DR2">
@@ -1810,7 +1818,7 @@
       <c r="AI3">
         <v>0</v>
       </c>
-      <c r="AJ3">
+      <c r="AJ3" s="1">
         <v>0</v>
       </c>
       <c r="AK3">
@@ -1828,7 +1836,7 @@
       <c r="AO3">
         <v>0</v>
       </c>
-      <c r="AP3">
+      <c r="AP3" s="1">
         <v>0</v>
       </c>
       <c r="AQ3">
@@ -1864,7 +1872,7 @@
       <c r="BA3">
         <v>0</v>
       </c>
-      <c r="BB3">
+      <c r="BB3" s="1">
         <v>0</v>
       </c>
       <c r="BC3">
@@ -1885,7 +1893,7 @@
       <c r="BH3">
         <v>0</v>
       </c>
-      <c r="BI3">
+      <c r="BI3" s="1">
         <v>0</v>
       </c>
       <c r="BJ3">
@@ -1906,7 +1914,7 @@
       <c r="BO3">
         <v>0</v>
       </c>
-      <c r="BP3">
+      <c r="BP3" s="2">
         <v>0</v>
       </c>
       <c r="BQ3">
@@ -1924,7 +1932,7 @@
       <c r="BU3">
         <v>0</v>
       </c>
-      <c r="BV3">
+      <c r="BV3" s="1">
         <v>0</v>
       </c>
       <c r="BW3">
@@ -1960,7 +1968,7 @@
       <c r="CG3">
         <v>0</v>
       </c>
-      <c r="CH3">
+      <c r="CH3" s="1">
         <v>0</v>
       </c>
       <c r="CI3">
@@ -1990,7 +1998,7 @@
       <c r="CQ3">
         <v>0</v>
       </c>
-      <c r="CR3">
+      <c r="CR3" s="1">
         <v>0</v>
       </c>
       <c r="CS3">
@@ -2026,7 +2034,7 @@
       <c r="DC3">
         <v>0</v>
       </c>
-      <c r="DD3">
+      <c r="DD3" s="1">
         <v>0</v>
       </c>
       <c r="DE3">
@@ -2065,7 +2073,7 @@
       <c r="DP3">
         <v>0</v>
       </c>
-      <c r="DQ3">
+      <c r="DQ3" s="1">
         <v>0</v>
       </c>
       <c r="DR3">
@@ -2196,7 +2204,7 @@
       <c r="AI4">
         <v>0</v>
       </c>
-      <c r="AJ4">
+      <c r="AJ4" s="1">
         <v>0</v>
       </c>
       <c r="AK4">
@@ -2214,7 +2222,7 @@
       <c r="AO4">
         <v>0</v>
       </c>
-      <c r="AP4">
+      <c r="AP4" s="1">
         <v>0</v>
       </c>
       <c r="AQ4">
@@ -2250,7 +2258,7 @@
       <c r="BA4">
         <v>0</v>
       </c>
-      <c r="BB4">
+      <c r="BB4" s="1">
         <v>0</v>
       </c>
       <c r="BC4">
@@ -2271,7 +2279,7 @@
       <c r="BH4">
         <v>0</v>
       </c>
-      <c r="BI4">
+      <c r="BI4" s="1">
         <v>0</v>
       </c>
       <c r="BJ4">
@@ -2292,7 +2300,7 @@
       <c r="BO4">
         <v>0</v>
       </c>
-      <c r="BP4">
+      <c r="BP4" s="2">
         <v>0</v>
       </c>
       <c r="BQ4">
@@ -2310,7 +2318,7 @@
       <c r="BU4">
         <v>0</v>
       </c>
-      <c r="BV4">
+      <c r="BV4" s="1">
         <v>0</v>
       </c>
       <c r="BW4">
@@ -2346,7 +2354,7 @@
       <c r="CG4">
         <v>0</v>
       </c>
-      <c r="CH4">
+      <c r="CH4" s="1">
         <v>0</v>
       </c>
       <c r="CI4">
@@ -2376,7 +2384,7 @@
       <c r="CQ4">
         <v>0</v>
       </c>
-      <c r="CR4">
+      <c r="CR4" s="1">
         <v>0</v>
       </c>
       <c r="CS4">
@@ -2412,7 +2420,7 @@
       <c r="DC4">
         <v>0</v>
       </c>
-      <c r="DD4">
+      <c r="DD4" s="1">
         <v>0</v>
       </c>
       <c r="DE4">
@@ -2451,7 +2459,7 @@
       <c r="DP4">
         <v>0</v>
       </c>
-      <c r="DQ4">
+      <c r="DQ4" s="1">
         <v>0</v>
       </c>
       <c r="DR4">
@@ -2582,7 +2590,7 @@
       <c r="AI5">
         <v>1</v>
       </c>
-      <c r="AJ5">
+      <c r="AJ5" s="1">
         <v>0</v>
       </c>
       <c r="AK5">
@@ -2600,7 +2608,7 @@
       <c r="AO5">
         <v>0</v>
       </c>
-      <c r="AP5">
+      <c r="AP5" s="1">
         <v>0</v>
       </c>
       <c r="AQ5">
@@ -2636,7 +2644,7 @@
       <c r="BA5">
         <v>0</v>
       </c>
-      <c r="BB5">
+      <c r="BB5" s="1">
         <v>0</v>
       </c>
       <c r="BC5">
@@ -2657,7 +2665,7 @@
       <c r="BH5">
         <v>0</v>
       </c>
-      <c r="BI5">
+      <c r="BI5" s="1">
         <v>0</v>
       </c>
       <c r="BJ5">
@@ -2678,7 +2686,7 @@
       <c r="BO5">
         <v>0</v>
       </c>
-      <c r="BP5">
+      <c r="BP5" s="2">
         <v>0</v>
       </c>
       <c r="BQ5">
@@ -2696,7 +2704,7 @@
       <c r="BU5">
         <v>0</v>
       </c>
-      <c r="BV5">
+      <c r="BV5" s="1">
         <v>0</v>
       </c>
       <c r="BW5">
@@ -2732,7 +2740,7 @@
       <c r="CG5">
         <v>0</v>
       </c>
-      <c r="CH5">
+      <c r="CH5" s="1">
         <v>0</v>
       </c>
       <c r="CI5">
@@ -2762,7 +2770,7 @@
       <c r="CQ5">
         <v>0</v>
       </c>
-      <c r="CR5">
+      <c r="CR5" s="1">
         <v>0</v>
       </c>
       <c r="CS5">
@@ -2798,7 +2806,7 @@
       <c r="DC5">
         <v>0</v>
       </c>
-      <c r="DD5">
+      <c r="DD5" s="1">
         <v>0</v>
       </c>
       <c r="DE5">
@@ -2837,7 +2845,7 @@
       <c r="DP5">
         <v>0</v>
       </c>
-      <c r="DQ5">
+      <c r="DQ5" s="1">
         <v>0</v>
       </c>
       <c r="DR5">
@@ -2968,7 +2976,7 @@
       <c r="AI6">
         <v>0</v>
       </c>
-      <c r="AJ6">
+      <c r="AJ6" s="1">
         <v>13</v>
       </c>
       <c r="AK6">
@@ -2986,7 +2994,7 @@
       <c r="AO6">
         <v>1</v>
       </c>
-      <c r="AP6">
+      <c r="AP6" s="1">
         <v>1</v>
       </c>
       <c r="AQ6">
@@ -3022,7 +3030,7 @@
       <c r="BA6">
         <v>0</v>
       </c>
-      <c r="BB6">
+      <c r="BB6" s="1">
         <v>0</v>
       </c>
       <c r="BC6">
@@ -3043,7 +3051,7 @@
       <c r="BH6">
         <v>0</v>
       </c>
-      <c r="BI6">
+      <c r="BI6" s="1">
         <v>0</v>
       </c>
       <c r="BJ6">
@@ -3064,7 +3072,7 @@
       <c r="BO6">
         <v>0</v>
       </c>
-      <c r="BP6">
+      <c r="BP6" s="2">
         <v>0</v>
       </c>
       <c r="BQ6">
@@ -3082,7 +3090,7 @@
       <c r="BU6">
         <v>0</v>
       </c>
-      <c r="BV6">
+      <c r="BV6" s="1">
         <v>0</v>
       </c>
       <c r="BW6">
@@ -3118,7 +3126,7 @@
       <c r="CG6">
         <v>0</v>
       </c>
-      <c r="CH6">
+      <c r="CH6" s="1">
         <v>0</v>
       </c>
       <c r="CI6">
@@ -3148,7 +3156,7 @@
       <c r="CQ6">
         <v>0</v>
       </c>
-      <c r="CR6">
+      <c r="CR6" s="1">
         <v>0</v>
       </c>
       <c r="CS6">
@@ -3184,7 +3192,7 @@
       <c r="DC6">
         <v>0</v>
       </c>
-      <c r="DD6">
+      <c r="DD6" s="1">
         <v>0</v>
       </c>
       <c r="DE6">
@@ -3223,7 +3231,7 @@
       <c r="DP6">
         <v>0</v>
       </c>
-      <c r="DQ6">
+      <c r="DQ6" s="1">
         <v>0</v>
       </c>
       <c r="DR6">
@@ -3354,7 +3362,7 @@
       <c r="AI7">
         <v>0</v>
       </c>
-      <c r="AJ7">
+      <c r="AJ7" s="1">
         <v>4</v>
       </c>
       <c r="AK7">
@@ -3372,7 +3380,7 @@
       <c r="AO7">
         <v>0</v>
       </c>
-      <c r="AP7">
+      <c r="AP7" s="1">
         <v>1</v>
       </c>
       <c r="AQ7">
@@ -3408,7 +3416,7 @@
       <c r="BA7">
         <v>1</v>
       </c>
-      <c r="BB7">
+      <c r="BB7" s="1">
         <v>1</v>
       </c>
       <c r="BC7">
@@ -3429,7 +3437,7 @@
       <c r="BH7">
         <v>0</v>
       </c>
-      <c r="BI7">
+      <c r="BI7" s="1">
         <v>0</v>
       </c>
       <c r="BJ7">
@@ -3450,7 +3458,7 @@
       <c r="BO7">
         <v>0</v>
       </c>
-      <c r="BP7">
+      <c r="BP7" s="2">
         <v>0</v>
       </c>
       <c r="BQ7">
@@ -3468,7 +3476,7 @@
       <c r="BU7">
         <v>0</v>
       </c>
-      <c r="BV7">
+      <c r="BV7" s="1">
         <v>0</v>
       </c>
       <c r="BW7">
@@ -3504,7 +3512,7 @@
       <c r="CG7">
         <v>0</v>
       </c>
-      <c r="CH7">
+      <c r="CH7" s="1">
         <v>0</v>
       </c>
       <c r="CI7">
@@ -3534,7 +3542,7 @@
       <c r="CQ7">
         <v>0</v>
       </c>
-      <c r="CR7">
+      <c r="CR7" s="1">
         <v>0</v>
       </c>
       <c r="CS7">
@@ -3570,7 +3578,7 @@
       <c r="DC7">
         <v>0</v>
       </c>
-      <c r="DD7">
+      <c r="DD7" s="1">
         <v>0</v>
       </c>
       <c r="DE7">
@@ -3609,7 +3617,7 @@
       <c r="DP7">
         <v>0</v>
       </c>
-      <c r="DQ7">
+      <c r="DQ7" s="1">
         <v>0</v>
       </c>
       <c r="DR7">
@@ -3740,7 +3748,7 @@
       <c r="AI8">
         <v>4</v>
       </c>
-      <c r="AJ8">
+      <c r="AJ8" s="1">
         <v>10</v>
       </c>
       <c r="AK8">
@@ -3758,7 +3766,7 @@
       <c r="AO8">
         <v>0</v>
       </c>
-      <c r="AP8">
+      <c r="AP8" s="1">
         <v>0</v>
       </c>
       <c r="AQ8">
@@ -3794,7 +3802,7 @@
       <c r="BA8">
         <v>0</v>
       </c>
-      <c r="BB8">
+      <c r="BB8" s="1">
         <v>1</v>
       </c>
       <c r="BC8">
@@ -3815,7 +3823,7 @@
       <c r="BH8">
         <v>2</v>
       </c>
-      <c r="BI8">
+      <c r="BI8" s="1">
         <v>2</v>
       </c>
       <c r="BJ8">
@@ -3836,7 +3844,7 @@
       <c r="BO8">
         <v>1</v>
       </c>
-      <c r="BP8">
+      <c r="BP8" s="2">
         <v>0</v>
       </c>
       <c r="BQ8">
@@ -3854,7 +3862,7 @@
       <c r="BU8">
         <v>0</v>
       </c>
-      <c r="BV8">
+      <c r="BV8" s="1">
         <v>0</v>
       </c>
       <c r="BW8">
@@ -3890,7 +3898,7 @@
       <c r="CG8">
         <v>0</v>
       </c>
-      <c r="CH8">
+      <c r="CH8" s="1">
         <v>0</v>
       </c>
       <c r="CI8">
@@ -3920,7 +3928,7 @@
       <c r="CQ8">
         <v>0</v>
       </c>
-      <c r="CR8">
+      <c r="CR8" s="1">
         <v>0</v>
       </c>
       <c r="CS8">
@@ -3956,7 +3964,7 @@
       <c r="DC8">
         <v>0</v>
       </c>
-      <c r="DD8">
+      <c r="DD8" s="1">
         <v>0</v>
       </c>
       <c r="DE8">
@@ -3995,7 +4003,7 @@
       <c r="DP8">
         <v>0</v>
       </c>
-      <c r="DQ8">
+      <c r="DQ8" s="1">
         <v>0</v>
       </c>
       <c r="DR8">
@@ -4126,7 +4134,7 @@
       <c r="AI9">
         <v>7</v>
       </c>
-      <c r="AJ9">
+      <c r="AJ9" s="1">
         <v>27</v>
       </c>
       <c r="AK9">
@@ -4144,7 +4152,7 @@
       <c r="AO9">
         <v>1</v>
       </c>
-      <c r="AP9">
+      <c r="AP9" s="1">
         <v>1</v>
       </c>
       <c r="AQ9">
@@ -4180,7 +4188,7 @@
       <c r="BA9">
         <v>3</v>
       </c>
-      <c r="BB9">
+      <c r="BB9" s="1">
         <v>7</v>
       </c>
       <c r="BC9">
@@ -4201,7 +4209,7 @@
       <c r="BH9">
         <v>0</v>
       </c>
-      <c r="BI9">
+      <c r="BI9" s="1">
         <v>7</v>
       </c>
       <c r="BJ9">
@@ -4222,7 +4230,7 @@
       <c r="BO9">
         <v>0</v>
       </c>
-      <c r="BP9">
+      <c r="BP9" s="2">
         <v>0</v>
       </c>
       <c r="BQ9">
@@ -4240,7 +4248,7 @@
       <c r="BU9">
         <v>2</v>
       </c>
-      <c r="BV9">
+      <c r="BV9" s="1">
         <v>2</v>
       </c>
       <c r="BW9">
@@ -4276,7 +4284,7 @@
       <c r="CG9">
         <v>1</v>
       </c>
-      <c r="CH9">
+      <c r="CH9" s="1">
         <v>1</v>
       </c>
       <c r="CI9">
@@ -4306,7 +4314,7 @@
       <c r="CQ9">
         <v>0</v>
       </c>
-      <c r="CR9">
+      <c r="CR9" s="1">
         <v>0</v>
       </c>
       <c r="CS9">
@@ -4342,7 +4350,7 @@
       <c r="DC9">
         <v>0</v>
       </c>
-      <c r="DD9">
+      <c r="DD9" s="1">
         <v>0</v>
       </c>
       <c r="DE9">
@@ -4381,7 +4389,7 @@
       <c r="DP9">
         <v>0</v>
       </c>
-      <c r="DQ9">
+      <c r="DQ9" s="1">
         <v>0</v>
       </c>
       <c r="DR9">
@@ -4512,7 +4520,7 @@
       <c r="AI10">
         <v>20</v>
       </c>
-      <c r="AJ10">
+      <c r="AJ10" s="1">
         <v>25</v>
       </c>
       <c r="AK10">
@@ -4530,7 +4538,7 @@
       <c r="AO10">
         <v>0</v>
       </c>
-      <c r="AP10">
+      <c r="AP10" s="1">
         <v>0</v>
       </c>
       <c r="AQ10">
@@ -4566,7 +4574,7 @@
       <c r="BA10">
         <v>10</v>
       </c>
-      <c r="BB10">
+      <c r="BB10" s="1">
         <v>9</v>
       </c>
       <c r="BC10">
@@ -4587,7 +4595,7 @@
       <c r="BH10">
         <v>3</v>
       </c>
-      <c r="BI10">
+      <c r="BI10" s="1">
         <v>9</v>
       </c>
       <c r="BJ10">
@@ -4608,7 +4616,7 @@
       <c r="BO10">
         <v>3</v>
       </c>
-      <c r="BP10">
+      <c r="BP10" s="2">
         <v>16</v>
       </c>
       <c r="BQ10">
@@ -4626,7 +4634,7 @@
       <c r="BU10">
         <v>1</v>
       </c>
-      <c r="BV10">
+      <c r="BV10" s="1">
         <v>3</v>
       </c>
       <c r="BW10">
@@ -4662,7 +4670,7 @@
       <c r="CG10">
         <v>0</v>
       </c>
-      <c r="CH10">
+      <c r="CH10" s="1">
         <v>1</v>
       </c>
       <c r="CI10">
@@ -4692,7 +4700,7 @@
       <c r="CQ10">
         <v>1</v>
       </c>
-      <c r="CR10">
+      <c r="CR10" s="1">
         <v>1</v>
       </c>
       <c r="CS10">
@@ -4728,7 +4736,7 @@
       <c r="DC10">
         <v>0</v>
       </c>
-      <c r="DD10">
+      <c r="DD10" s="1">
         <v>0</v>
       </c>
       <c r="DE10">
@@ -4767,7 +4775,7 @@
       <c r="DP10">
         <v>0</v>
       </c>
-      <c r="DQ10">
+      <c r="DQ10" s="1">
         <v>0</v>
       </c>
       <c r="DR10">
@@ -4898,7 +4906,7 @@
       <c r="AI11">
         <v>16</v>
       </c>
-      <c r="AJ11">
+      <c r="AJ11" s="1">
         <v>23</v>
       </c>
       <c r="AK11">
@@ -4916,7 +4924,7 @@
       <c r="AO11">
         <v>3</v>
       </c>
-      <c r="AP11">
+      <c r="AP11" s="1">
         <v>1</v>
       </c>
       <c r="AQ11">
@@ -4952,7 +4960,7 @@
       <c r="BA11">
         <v>1</v>
       </c>
-      <c r="BB11">
+      <c r="BB11" s="1">
         <v>12</v>
       </c>
       <c r="BC11">
@@ -4973,7 +4981,7 @@
       <c r="BH11">
         <v>2</v>
       </c>
-      <c r="BI11">
+      <c r="BI11" s="1">
         <v>9</v>
       </c>
       <c r="BJ11">
@@ -4994,7 +5002,7 @@
       <c r="BO11">
         <v>2</v>
       </c>
-      <c r="BP11">
+      <c r="BP11" s="2">
         <v>25</v>
       </c>
       <c r="BQ11">
@@ -5012,7 +5020,7 @@
       <c r="BU11">
         <v>2</v>
       </c>
-      <c r="BV11">
+      <c r="BV11" s="1">
         <v>3</v>
       </c>
       <c r="BW11">
@@ -5048,7 +5056,7 @@
       <c r="CG11">
         <v>0</v>
       </c>
-      <c r="CH11">
+      <c r="CH11" s="1">
         <v>1</v>
       </c>
       <c r="CI11">
@@ -5078,7 +5086,7 @@
       <c r="CQ11">
         <v>0</v>
       </c>
-      <c r="CR11">
+      <c r="CR11" s="1">
         <v>4</v>
       </c>
       <c r="CS11">
@@ -5114,7 +5122,7 @@
       <c r="DC11">
         <v>1</v>
       </c>
-      <c r="DD11">
+      <c r="DD11" s="1">
         <v>1</v>
       </c>
       <c r="DE11">
@@ -5153,7 +5161,7 @@
       <c r="DP11">
         <v>0</v>
       </c>
-      <c r="DQ11">
+      <c r="DQ11" s="1">
         <v>0</v>
       </c>
       <c r="DR11">
@@ -5284,7 +5292,7 @@
       <c r="AI12">
         <v>11</v>
       </c>
-      <c r="AJ12">
+      <c r="AJ12" s="1">
         <v>25</v>
       </c>
       <c r="AK12">
@@ -5302,7 +5310,7 @@
       <c r="AO12">
         <v>0</v>
       </c>
-      <c r="AP12">
+      <c r="AP12" s="1">
         <v>4</v>
       </c>
       <c r="AQ12">
@@ -5338,7 +5346,7 @@
       <c r="BA12">
         <v>5</v>
       </c>
-      <c r="BB12">
+      <c r="BB12" s="1">
         <v>8</v>
       </c>
       <c r="BC12">
@@ -5359,7 +5367,7 @@
       <c r="BH12">
         <v>6</v>
       </c>
-      <c r="BI12">
+      <c r="BI12" s="1">
         <v>12</v>
       </c>
       <c r="BJ12">
@@ -5380,7 +5388,7 @@
       <c r="BO12">
         <v>2</v>
       </c>
-      <c r="BP12">
+      <c r="BP12" s="2">
         <v>27</v>
       </c>
       <c r="BQ12">
@@ -5398,7 +5406,7 @@
       <c r="BU12">
         <v>4</v>
       </c>
-      <c r="BV12">
+      <c r="BV12" s="1">
         <v>5</v>
       </c>
       <c r="BW12">
@@ -5434,7 +5442,7 @@
       <c r="CG12">
         <v>1</v>
       </c>
-      <c r="CH12">
+      <c r="CH12" s="1">
         <v>1</v>
       </c>
       <c r="CI12">
@@ -5464,7 +5472,7 @@
       <c r="CQ12">
         <v>0</v>
       </c>
-      <c r="CR12">
+      <c r="CR12" s="1">
         <v>1</v>
       </c>
       <c r="CS12">
@@ -5500,7 +5508,7 @@
       <c r="DC12">
         <v>0</v>
       </c>
-      <c r="DD12">
+      <c r="DD12" s="1">
         <v>0</v>
       </c>
       <c r="DE12">
@@ -5539,7 +5547,7 @@
       <c r="DP12">
         <v>0</v>
       </c>
-      <c r="DQ12">
+      <c r="DQ12" s="1">
         <v>0</v>
       </c>
       <c r="DR12">
@@ -5670,7 +5678,7 @@
       <c r="AI13">
         <v>12</v>
       </c>
-      <c r="AJ13">
+      <c r="AJ13" s="1">
         <v>20</v>
       </c>
       <c r="AK13">
@@ -5688,7 +5696,7 @@
       <c r="AO13">
         <v>0</v>
       </c>
-      <c r="AP13">
+      <c r="AP13" s="1">
         <v>6</v>
       </c>
       <c r="AQ13">
@@ -5724,7 +5732,7 @@
       <c r="BA13">
         <v>8</v>
       </c>
-      <c r="BB13">
+      <c r="BB13" s="1">
         <v>12</v>
       </c>
       <c r="BC13">
@@ -5745,7 +5753,7 @@
       <c r="BH13">
         <v>4</v>
       </c>
-      <c r="BI13">
+      <c r="BI13" s="1">
         <v>14</v>
       </c>
       <c r="BJ13">
@@ -5766,7 +5774,7 @@
       <c r="BO13">
         <v>8</v>
       </c>
-      <c r="BP13">
+      <c r="BP13" s="2">
         <v>38</v>
       </c>
       <c r="BQ13">
@@ -5784,7 +5792,7 @@
       <c r="BU13">
         <v>10</v>
       </c>
-      <c r="BV13">
+      <c r="BV13" s="1">
         <v>7</v>
       </c>
       <c r="BW13">
@@ -5820,7 +5828,7 @@
       <c r="CG13">
         <v>0</v>
       </c>
-      <c r="CH13">
+      <c r="CH13" s="1">
         <v>4</v>
       </c>
       <c r="CI13">
@@ -5850,7 +5858,7 @@
       <c r="CQ13">
         <v>0</v>
       </c>
-      <c r="CR13">
+      <c r="CR13" s="1">
         <v>9</v>
       </c>
       <c r="CS13">
@@ -5886,7 +5894,7 @@
       <c r="DC13">
         <v>0</v>
       </c>
-      <c r="DD13">
+      <c r="DD13" s="1">
         <v>0</v>
       </c>
       <c r="DE13">
@@ -5925,7 +5933,7 @@
       <c r="DP13">
         <v>1</v>
       </c>
-      <c r="DQ13">
+      <c r="DQ13" s="1">
         <v>1</v>
       </c>
       <c r="DR13">
@@ -6056,7 +6064,7 @@
       <c r="AI14">
         <v>13</v>
       </c>
-      <c r="AJ14">
+      <c r="AJ14" s="1">
         <v>26</v>
       </c>
       <c r="AK14">
@@ -6074,7 +6082,7 @@
       <c r="AO14">
         <v>1</v>
       </c>
-      <c r="AP14">
+      <c r="AP14" s="1">
         <v>2</v>
       </c>
       <c r="AQ14">
@@ -6110,7 +6118,7 @@
       <c r="BA14">
         <v>7</v>
       </c>
-      <c r="BB14">
+      <c r="BB14" s="1">
         <v>15</v>
       </c>
       <c r="BC14">
@@ -6131,7 +6139,7 @@
       <c r="BH14">
         <v>7</v>
       </c>
-      <c r="BI14">
+      <c r="BI14" s="1">
         <v>20</v>
       </c>
       <c r="BJ14">
@@ -6152,7 +6160,7 @@
       <c r="BO14">
         <v>3</v>
       </c>
-      <c r="BP14">
+      <c r="BP14" s="2">
         <v>41</v>
       </c>
       <c r="BQ14">
@@ -6170,7 +6178,7 @@
       <c r="BU14">
         <v>14</v>
       </c>
-      <c r="BV14">
+      <c r="BV14" s="1">
         <v>7</v>
       </c>
       <c r="BW14">
@@ -6206,7 +6214,7 @@
       <c r="CG14">
         <v>1</v>
       </c>
-      <c r="CH14">
+      <c r="CH14" s="1">
         <v>4</v>
       </c>
       <c r="CI14">
@@ -6236,7 +6244,7 @@
       <c r="CQ14">
         <v>0</v>
       </c>
-      <c r="CR14">
+      <c r="CR14" s="1">
         <v>9</v>
       </c>
       <c r="CS14">
@@ -6272,7 +6280,7 @@
       <c r="DC14">
         <v>0</v>
       </c>
-      <c r="DD14">
+      <c r="DD14" s="1">
         <v>0</v>
       </c>
       <c r="DE14">
@@ -6311,7 +6319,7 @@
       <c r="DP14">
         <v>1</v>
       </c>
-      <c r="DQ14">
+      <c r="DQ14" s="1">
         <v>0</v>
       </c>
       <c r="DR14">

</xml_diff>